<commit_message>
undo delete bias and resources required doing 611
</commit_message>
<xml_diff>
--- a/2026-TERM1/T1B1-BSBCRT611_Apply_critical_thinking_for_complex_problem_solving/2-assessments/graph-excel.xlsx
+++ b/2026-TERM1/T1B1-BSBCRT611_Apply_critical_thinking_for_complex_problem_solving/2-assessments/graph-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mannsee/Documents/Assessments/2026-TERM1/T1B1-BSBCRT611_Apply_critical_thinking_for_complex_problem_solving/2-assessments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB02B02B-DEA8-8C46-8A9B-06483067E300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E64FEB-BDD7-EB41-9510-A0D3FB3E7C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="10020" windowHeight="18980" activeTab="6" xr2:uid="{E87DA1E5-4B9A-F64B-9951-0716BE63B2DA}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="10020" windowHeight="18980" firstSheet="4" activeTab="6" xr2:uid="{E87DA1E5-4B9A-F64B-9951-0716BE63B2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="stakeholders" sheetId="1" r:id="rId1"/>

</xml_diff>